<commit_message>
The following has been changed
</commit_message>
<xml_diff>
--- a/Resources/Data/SampleData.xlsx
+++ b/Resources/Data/SampleData.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contacts data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,62 +443,320 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>FirstName</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>LastName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>AccountId</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>30</v>
+          <t>0038N00000D0REQQA3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jon</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Amos</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>(905) 555-1212</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhEQAV</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jane</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>25</v>
+          <t>0038N00000D0RERQA3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>john@servicecloud.trial</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(212) 555-5555</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhFQAV</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>35</v>
+          <t>0038N00000D0RESQA3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Geoff</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Minor</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>(415) 555-1212</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhEQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0038N00000D0RETQA3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Carole</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>(415) 555-1212</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhEQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0038N00000D0REUQA3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Edward</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Stamos</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>(212) 555-5555</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhFQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0038N00000D0REVQA3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Howard</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Jones</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>(212) 555-5555</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhFQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0038N00000D0REWQA3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Leanne</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tomlin</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>(212) 555-5555</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhFQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0038N00000D0REXQA3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Marc</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Benioff</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>info@salesforce.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>(415) 901-7000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhGQAV</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0038N00000D0REYQA3</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Land</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>your.email@test.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>(415) 555-5555</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0018N00000EyKhFQAV</t>
         </is>
       </c>
     </row>

</xml_diff>